<commit_message>
using 0507 version benchmark report
</commit_message>
<xml_diff>
--- a/lib/report/benchmark_report/web14/exl/201912/jsliu__bank_test_&_city_(HF)(201912)_KRD.xlsx
+++ b/lib/report/benchmark_report/web14/exl/201912/jsliu__bank_test_&_city_(HF)(201912)_KRD.xlsx
@@ -39,7 +39,7 @@
     <t xml:space="preserve">Cycle: December, 2019        Evaluation Date: December 31, 2019</t>
   </si>
   <si>
-    <t>Printed on: 04/16/20 2:14:52 PM</t>
+    <t>Printed on: 05/02/20 4:48:01 AM</t>
   </si>
   <si>
     <t>Comments:</t>
@@ -3928,37 +3928,37 @@
         <v>18</v>
       </c>
       <c r="B7" s="236">
-        <v>112153.55805661147</v>
+        <v>112153.55805661112</v>
       </c>
       <c r="C7" s="236">
-        <v>0.050858588986229615</v>
+        <v>0.050858588986359525</v>
       </c>
       <c r="D7" s="236">
-        <v>0.38269886764937144</v>
+        <v>0.38269886764924288</v>
       </c>
       <c r="E7" s="236">
-        <v>0.77327348716380084</v>
+        <v>0.77327348716360855</v>
       </c>
       <c r="F7" s="236">
-        <v>0.4532275145766882</v>
+        <v>0.45322751457681937</v>
       </c>
       <c r="G7" s="236">
-        <v>0.28160964060253363</v>
+        <v>0.28160964060298865</v>
       </c>
       <c r="H7" s="236">
-        <v>0.43211715770912851</v>
+        <v>0.43211715770718362</v>
       </c>
       <c r="I7" s="236">
-        <v>0.069859296389232717</v>
+        <v>0.069859296389622183</v>
       </c>
       <c r="J7" s="236">
-        <v>0.010566490683961823</v>
+        <v>0.010566490684091604</v>
       </c>
       <c r="K7" s="236">
-        <v>2.450699984151254</v>
+        <v>2.450699984148407</v>
       </c>
       <c r="L7" s="236">
-        <v>0.052130450739404</v>
+        <v>0.052130450757569148</v>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1">
@@ -3966,37 +3966,37 @@
         <v>19</v>
       </c>
       <c r="B8" s="236">
-        <v>90250.489588777986</v>
+        <v>90250.489588782017</v>
       </c>
       <c r="C8" s="236">
-        <v>0.04234615138376354</v>
+        <v>0.042346151383842269</v>
       </c>
       <c r="D8" s="236">
-        <v>0.33191234464942593</v>
+        <v>0.33191234464957237</v>
       </c>
       <c r="E8" s="236">
-        <v>0.3351301935716775</v>
+        <v>0.33513019357359741</v>
       </c>
       <c r="F8" s="236">
-        <v>0.21292934826468141</v>
+        <v>0.21292934826475252</v>
       </c>
       <c r="G8" s="236">
-        <v>0.13321677587998199</v>
+        <v>0.13321677587973416</v>
       </c>
       <c r="H8" s="236">
-        <v>0.14852654426292022</v>
+        <v>0.14852654426242987</v>
       </c>
       <c r="I8" s="236">
-        <v>0.060631575175178982</v>
+        <v>0.060631575175659994</v>
       </c>
       <c r="J8" s="236">
-        <v>0.013614101081019174</v>
+        <v>0.013614101079970511</v>
       </c>
       <c r="K8" s="236">
-        <v>1.2782036289641694</v>
+        <v>1.2782036289653216</v>
       </c>
       <c r="L8" s="236">
-        <v>0.07491584567009435</v>
+        <v>0.074915845665253819</v>
       </c>
     </row>
     <row r="9" hidden="1" ht="15" customHeight="1">
@@ -4018,37 +4018,37 @@
         <v>20</v>
       </c>
       <c r="B10" s="236">
-        <v>21903.068467833476</v>
+        <v>21903.068467829104</v>
       </c>
       <c r="C10" s="236">
-        <v>0.085933659054201708</v>
+        <v>0.085933659054883232</v>
       </c>
       <c r="D10" s="236">
-        <v>0.59196217575546872</v>
+        <v>0.59196217575459031</v>
       </c>
       <c r="E10" s="236">
-        <v>2.5786208436221241</v>
+        <v>2.578620843613753</v>
       </c>
       <c r="F10" s="236">
-        <v>1.4433639965398435</v>
+        <v>1.4433639965405469</v>
       </c>
       <c r="G10" s="236">
-        <v>0.89305495989025341</v>
+        <v>0.89305495989350447</v>
       </c>
       <c r="H10" s="236">
-        <v>1.6006379859160564</v>
+        <v>1.6006379859085695</v>
       </c>
       <c r="I10" s="236">
-        <v>0.1078816565247612</v>
+        <v>0.1078816565243675</v>
       </c>
       <c r="J10" s="236">
-        <v>-0.0019910343409254459</v>
+        <v>-0.0019910343361921505</v>
       </c>
       <c r="K10" s="236">
-        <v>7.2819121155517195</v>
+        <v>7.2819121155334079</v>
       </c>
       <c r="L10" s="236">
-        <v>-0.04175562056555733</v>
+        <v>-0.041755620455943311</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1">
@@ -4175,28 +4175,28 @@
         <v>32</v>
       </c>
       <c r="D40" s="236">
-        <v>7870.0312267641448</v>
+        <v>7870.03122682499</v>
       </c>
       <c r="E40" s="236">
-        <v>12997.483302719453</v>
+        <v>12997.483302697572</v>
       </c>
       <c r="F40" s="236">
-        <v>18873.915750100005</v>
+        <v>18873.915750034965</v>
       </c>
       <c r="G40" s="236">
-        <v>6349.4050799922234</v>
+        <v>6349.40507999405</v>
       </c>
       <c r="H40" s="236">
-        <v>2810.6116958587372</v>
+        <v>2810.6116958684079</v>
       </c>
       <c r="I40" s="236">
-        <v>3536.3591117252331</v>
+        <v>3536.3591117079859</v>
       </c>
       <c r="J40" s="236">
-        <v>119.6209532235337</v>
+        <v>119.62095322307329</v>
       </c>
       <c r="K40" s="236">
-        <v>-1.4751281891640766</v>
+        <v>-1.4751281856569527</v>
       </c>
     </row>
     <row r="41" ht="15" customHeight="1">
@@ -4204,28 +4204,28 @@
         <v>33</v>
       </c>
       <c r="D41" s="236">
-        <v>122.58543999596972</v>
+        <v>122.58543999691746</v>
       </c>
       <c r="E41" s="236">
-        <v>206.40517966463241</v>
+        <v>206.40517966428493</v>
       </c>
       <c r="F41" s="236">
-        <v>322.57505401222568</v>
+        <v>322.5750540111141</v>
       </c>
       <c r="G41" s="236">
-        <v>117.100043818959</v>
+        <v>117.10004381899269</v>
       </c>
       <c r="H41" s="236">
-        <v>62.42199379049481</v>
+        <v>62.421993790709585</v>
       </c>
       <c r="I41" s="236">
-        <v>77.692433873097954</v>
+        <v>77.692433872719036</v>
       </c>
       <c r="J41" s="236">
-        <v>3.4517251854743978</v>
+        <v>3.451725185461112</v>
       </c>
       <c r="K41" s="236">
-        <v>-0.041475517671419174</v>
+        <v>-0.041475517572810941</v>
       </c>
     </row>
     <row r="42" ht="15" customHeight="1">
@@ -4233,7 +4233,7 @@
         <v>34</v>
       </c>
       <c r="D42" s="236">
-        <v>912.19039482318249</v>
+        <v>912.1903948226261</v>
       </c>
       <c r="E42" s="236">
         <v>0</v>
@@ -4306,28 +4306,28 @@
         <v>44</v>
       </c>
       <c r="D46" s="236">
-        <v>23239.859783151413</v>
+        <v>23239.859783135737</v>
       </c>
       <c r="E46" s="236">
-        <v>22636.93852795097</v>
+        <v>22636.938527937189</v>
       </c>
       <c r="F46" s="236">
-        <v>21903.068467833476</v>
+        <v>21903.068467829104</v>
       </c>
       <c r="G46" s="236">
-        <v>21099.691031926643</v>
+        <v>21099.691031922939</v>
       </c>
       <c r="H46" s="236">
-        <v>20368.193557389375</v>
+        <v>20368.19355736579</v>
       </c>
       <c r="I46" s="236">
-        <v>18988.452346157406</v>
+        <v>18988.452346151931</v>
       </c>
       <c r="J46" s="236">
-        <v>16411.956351878704</v>
+        <v>16411.956351877019</v>
       </c>
       <c r="K46" s="236">
-        <v>13484.920157567549</v>
+        <v>13484.920157566734</v>
       </c>
     </row>
     <row r="47" ht="15" customHeight="1">
@@ -4335,28 +4335,28 @@
         <v>45</v>
       </c>
       <c r="D47" s="236">
-        <v>23544.940337859178</v>
+        <v>23544.94033785287</v>
       </c>
       <c r="E47" s="236">
-        <v>22711.70582228222</v>
+        <v>22711.705822276865</v>
       </c>
       <c r="F47" s="236">
-        <v>21903.068467833476</v>
+        <v>21903.068467829107</v>
       </c>
       <c r="G47" s="236">
-        <v>21118.012511477831</v>
+        <v>21118.012511474473</v>
       </c>
       <c r="H47" s="236">
-        <v>20355.575299110973</v>
+        <v>20355.575299108641</v>
       </c>
       <c r="I47" s="236">
-        <v>18894.952268499004</v>
+        <v>18894.952268498761</v>
       </c>
       <c r="J47" s="236">
-        <v>17514.439504668786</v>
+        <v>17514.439504670619</v>
       </c>
       <c r="K47" s="236">
-        <v>16207.936997572531</v>
+        <v>16207.93699757642</v>
       </c>
     </row>
     <row r="48" hidden="1" ht="15" customHeight="1">
@@ -4377,28 +4377,28 @@
         <v>47</v>
       </c>
       <c r="D49" s="236">
-        <v>1.3127469681591821</v>
+        <v>1.312746968200377</v>
       </c>
       <c r="E49" s="236">
-        <v>0.33028889590759397</v>
+        <v>0.33028889594501543</v>
       </c>
       <c r="F49" s="236">
-        <v>0</v>
+        <v>1.6609448180446138E-14</v>
       </c>
       <c r="G49" s="236">
-        <v>0.086832928138453266</v>
+        <v>0.086832928140106486</v>
       </c>
       <c r="H49" s="236">
-        <v>-0.061950797172311986</v>
+        <v>-0.061950797068039312</v>
       </c>
       <c r="I49" s="236">
-        <v>-0.49240494145550057</v>
+        <v>-0.4924049414280921</v>
       </c>
       <c r="J49" s="236">
-        <v>6.7175608388934052</v>
+        <v>6.7175608389155288</v>
       </c>
       <c r="K49" s="236">
-        <v>20.193051261611387</v>
+        <v>20.193051261647494</v>
       </c>
     </row>
     <row r="50" hidden="1" ht="15" customHeight="1">
@@ -4549,25 +4549,25 @@
         <v>53</v>
       </c>
       <c r="B75" s="261">
-        <v>3234.73308532013</v>
+        <v>3234.73308532061</v>
       </c>
       <c r="C75" s="261">
-        <v>0.00666143681610679</v>
+        <v>0.0066614368146296846</v>
       </c>
       <c r="D75" s="261">
-        <v>0.058453682125507424</v>
+        <v>0.058453682125358168</v>
       </c>
       <c r="E75" s="261">
-        <v>1.5959601605997633</v>
+        <v>1.5959601605995266</v>
       </c>
       <c r="F75" s="261">
-        <v>0.64956637510536785</v>
+        <v>0.64956637510534176</v>
       </c>
       <c r="G75" s="261">
-        <v>0.15156160399133759</v>
+        <v>0.1515616039912448</v>
       </c>
       <c r="H75" s="261">
-        <v>2.4457252895973851</v>
+        <v>2.4457252895986392</v>
       </c>
       <c r="I75" s="261">
         <v>0</v>
@@ -4576,10 +4576,10 @@
         <v>0</v>
       </c>
       <c r="K75" s="261">
-        <v>4.9079307097355436</v>
+        <v>4.9079307097362914</v>
       </c>
       <c r="L75" s="261">
-        <v>0.35736044437268305</v>
+        <v>0.35736044440496406</v>
       </c>
     </row>
     <row r="76" outlineLevel="2">
@@ -4587,25 +4587,25 @@
         <v>54</v>
       </c>
       <c r="B76" s="263">
-        <v>3234.73308532013</v>
+        <v>3234.73308532061</v>
       </c>
       <c r="C76" s="263">
-        <v>0.00666143681610679</v>
+        <v>0.0066614368146296846</v>
       </c>
       <c r="D76" s="263">
-        <v>0.058453682125507424</v>
+        <v>0.058453682125358168</v>
       </c>
       <c r="E76" s="263">
-        <v>1.5959601605997633</v>
+        <v>1.5959601605995266</v>
       </c>
       <c r="F76" s="263">
-        <v>0.64956637510536785</v>
+        <v>0.64956637510534176</v>
       </c>
       <c r="G76" s="263">
-        <v>0.15156160399133759</v>
+        <v>0.1515616039912448</v>
       </c>
       <c r="H76" s="263">
-        <v>2.4457252895973851</v>
+        <v>2.4457252895986392</v>
       </c>
       <c r="I76" s="263">
         <v>0</v>
@@ -4614,10 +4614,10 @@
         <v>0</v>
       </c>
       <c r="K76" s="263">
-        <v>4.9079307097355436</v>
+        <v>4.9079307097362914</v>
       </c>
       <c r="L76" s="263">
-        <v>0.35736044437268305</v>
+        <v>0.35736044440496406</v>
       </c>
     </row>
     <row r="77" outlineLevel="2">
@@ -4625,25 +4625,25 @@
         <v>55</v>
       </c>
       <c r="B77" s="261">
-        <v>1055.73318024361</v>
+        <v>1055.73318024377</v>
       </c>
       <c r="C77" s="261">
-        <v>0.0055664813941413756</v>
+        <v>0.0055664813987709953</v>
       </c>
       <c r="D77" s="261">
-        <v>0.048845518337499207</v>
+        <v>0.048845518342122266</v>
       </c>
       <c r="E77" s="261">
-        <v>1.6221884438639684</v>
+        <v>1.6221884438589844</v>
       </c>
       <c r="F77" s="261">
-        <v>0.6493691506947552</v>
+        <v>0.649369150694549</v>
       </c>
       <c r="G77" s="261">
-        <v>0.12664947517250494</v>
+        <v>0.12664947517248573</v>
       </c>
       <c r="H77" s="261">
-        <v>2.4994948959084318</v>
+        <v>2.499494895907945</v>
       </c>
       <c r="I77" s="261">
         <v>0</v>
@@ -4652,10 +4652,10 @@
         <v>0</v>
       </c>
       <c r="K77" s="261">
-        <v>4.9521157797927104</v>
+        <v>4.9521157797918525</v>
       </c>
       <c r="L77" s="261">
-        <v>0.36184950406974559</v>
+        <v>0.361849504067537</v>
       </c>
     </row>
     <row r="78" outlineLevel="2">
@@ -4663,37 +4663,37 @@
         <v>56</v>
       </c>
       <c r="B78" s="261">
-        <v>1574.2242352335984</v>
+        <v>1574.2242352335809</v>
       </c>
       <c r="C78" s="261">
-        <v>0.020270404638567153</v>
+        <v>0.020270404638567378</v>
       </c>
       <c r="D78" s="261">
-        <v>0.1917343784478017</v>
+        <v>0.19173437844780383</v>
       </c>
       <c r="E78" s="261">
-        <v>0.52174102337658479</v>
+        <v>0.52174102337976813</v>
       </c>
       <c r="F78" s="261">
-        <v>0.78220740055322724</v>
+        <v>0.78220740055641358</v>
       </c>
       <c r="G78" s="261">
-        <v>1.1194027247226797</v>
+        <v>1.1194027247258698</v>
       </c>
       <c r="H78" s="261">
-        <v>2.1318457819936643</v>
+        <v>2.1318457819841554</v>
       </c>
       <c r="I78" s="261">
-        <v>1.586915237275166</v>
+        <v>1.5869152372720061</v>
       </c>
       <c r="J78" s="261">
-        <v>0.46148877788194287</v>
+        <v>0.46148877787877041</v>
       </c>
       <c r="K78" s="261">
-        <v>6.8145044690048042</v>
+        <v>6.814504468995275</v>
       </c>
       <c r="L78" s="261">
-        <v>-0.39915335480040237</v>
+        <v>-0.399153354862514</v>
       </c>
     </row>
     <row r="79" outlineLevel="2">
@@ -4701,37 +4701,37 @@
         <v>57</v>
       </c>
       <c r="B79" s="263">
-        <v>1574.2242352335984</v>
+        <v>1574.2242352335809</v>
       </c>
       <c r="C79" s="263">
-        <v>0.020270404638567153</v>
+        <v>0.020270404638567378</v>
       </c>
       <c r="D79" s="263">
-        <v>0.1917343784478017</v>
+        <v>0.19173437844780383</v>
       </c>
       <c r="E79" s="263">
-        <v>0.52174102337658479</v>
+        <v>0.52174102337976813</v>
       </c>
       <c r="F79" s="263">
-        <v>0.78220740055322724</v>
+        <v>0.78220740055641358</v>
       </c>
       <c r="G79" s="263">
-        <v>1.1194027247226797</v>
+        <v>1.1194027247258698</v>
       </c>
       <c r="H79" s="263">
-        <v>2.1318457819936643</v>
+        <v>2.1318457819841554</v>
       </c>
       <c r="I79" s="263">
-        <v>1.586915237275166</v>
+        <v>1.5869152372720061</v>
       </c>
       <c r="J79" s="263">
-        <v>0.46148877788194287</v>
+        <v>0.46148877787877041</v>
       </c>
       <c r="K79" s="263">
-        <v>6.8145044690048042</v>
+        <v>6.814504468995275</v>
       </c>
       <c r="L79" s="263">
-        <v>-0.39915335480040237</v>
+        <v>-0.399153354862514</v>
       </c>
     </row>
     <row r="80" outlineLevel="2">
@@ -4739,25 +4739,25 @@
         <v>58</v>
       </c>
       <c r="B80" s="261">
-        <v>308.470953202964</v>
+        <v>308.47095320301</v>
       </c>
       <c r="C80" s="261">
-        <v>0.00483835935439984</v>
+        <v>0.0048383593543991172</v>
       </c>
       <c r="D80" s="261">
-        <v>0.04233984762387602</v>
+        <v>0.042339847625436036</v>
       </c>
       <c r="E80" s="261">
-        <v>1.6651368752945699</v>
+        <v>1.6651368752942291</v>
       </c>
       <c r="F80" s="261">
-        <v>0.65165716194911516</v>
+        <v>0.6516571619474516</v>
       </c>
       <c r="G80" s="261">
-        <v>0.10609386253125407</v>
+        <v>0.10609386253123823</v>
       </c>
       <c r="H80" s="261">
-        <v>2.4348625810298503</v>
+        <v>2.4348625810311453</v>
       </c>
       <c r="I80" s="261">
         <v>0</v>
@@ -4766,10 +4766,10 @@
         <v>0</v>
       </c>
       <c r="K80" s="261">
-        <v>4.9049302058417</v>
+        <v>4.9049302058409676</v>
       </c>
       <c r="L80" s="261">
-        <v>0.35418672638726406</v>
+        <v>0.35418672638352572</v>
       </c>
     </row>
     <row r="81" outlineLevel="2">
@@ -4777,25 +4777,25 @@
         <v>59</v>
       </c>
       <c r="B81" s="263">
-        <v>308.470953202964</v>
+        <v>308.47095320301</v>
       </c>
       <c r="C81" s="263">
-        <v>0.00483835935439984</v>
+        <v>0.0048383593543991172</v>
       </c>
       <c r="D81" s="263">
-        <v>0.04233984762387602</v>
+        <v>0.042339847625436036</v>
       </c>
       <c r="E81" s="263">
-        <v>1.6651368752945699</v>
+        <v>1.6651368752942291</v>
       </c>
       <c r="F81" s="263">
-        <v>0.65165716194911516</v>
+        <v>0.6516571619474516</v>
       </c>
       <c r="G81" s="263">
-        <v>0.10609386253125407</v>
+        <v>0.10609386253123823</v>
       </c>
       <c r="H81" s="263">
-        <v>2.4348625810298503</v>
+        <v>2.4348625810311453</v>
       </c>
       <c r="I81" s="263">
         <v>0</v>
@@ -4804,10 +4804,10 @@
         <v>0</v>
       </c>
       <c r="K81" s="263">
-        <v>4.9049302058417</v>
+        <v>4.9049302058409676</v>
       </c>
       <c r="L81" s="263">
-        <v>0.35418672638726406</v>
+        <v>0.35418672638352572</v>
       </c>
     </row>
     <row r="82" outlineLevel="2">
@@ -4815,37 +4815,37 @@
         <v>60</v>
       </c>
       <c r="B82" s="263">
-        <v>1882.6951884365624</v>
+        <v>1882.695188436591</v>
       </c>
       <c r="C82" s="263">
-        <v>0.017741934948972884</v>
+        <v>0.017741934949033002</v>
       </c>
       <c r="D82" s="263">
-        <v>0.16725677123359725</v>
+        <v>0.16725677123383625</v>
       </c>
       <c r="E82" s="263">
-        <v>0.70908117832874873</v>
+        <v>0.70908117833127415</v>
       </c>
       <c r="F82" s="263">
-        <v>0.76081734400532941</v>
+        <v>0.76081734400767287</v>
       </c>
       <c r="G82" s="263">
-        <v>0.95337672511902494</v>
+        <v>0.95337672512166738</v>
       </c>
       <c r="H82" s="263">
-        <v>2.1814936917611485</v>
+        <v>2.1814936917533858</v>
       </c>
       <c r="I82" s="263">
-        <v>1.3269064695781043</v>
+        <v>1.3269064695754271</v>
       </c>
       <c r="J82" s="263">
-        <v>0.3858759627644604</v>
+        <v>0.38587596276191838</v>
       </c>
       <c r="K82" s="263">
-        <v>6.50162950295196</v>
+        <v>6.5016295029439517</v>
       </c>
       <c r="L82" s="263">
-        <v>-0.27572204507100589</v>
+        <v>-0.27572204512534831</v>
       </c>
     </row>
     <row r="83" outlineLevel="1">
@@ -4853,37 +4853,37 @@
         <v>61</v>
       </c>
       <c r="B83" s="263">
-        <v>6173.161454000302</v>
+        <v>6173.1614540009714</v>
       </c>
       <c r="C83" s="263">
-        <v>0.00985351593104962</v>
+        <v>0.009853515931122216</v>
       </c>
       <c r="D83" s="263">
-        <v>0.089993339153684682</v>
+        <v>0.089993339154411572</v>
       </c>
       <c r="E83" s="263">
-        <v>1.3299647324904809</v>
+        <v>1.3299647324904103</v>
       </c>
       <c r="F83" s="263">
-        <v>0.68346204575353253</v>
+        <v>0.68346204575426872</v>
       </c>
       <c r="G83" s="263">
-        <v>0.391839283529043</v>
+        <v>0.39183928352966352</v>
       </c>
       <c r="H83" s="263">
-        <v>2.3743354185091627</v>
+        <v>2.3743354185074321</v>
       </c>
       <c r="I83" s="263">
-        <v>0.40468088262314877</v>
+        <v>0.40468088262236823</v>
       </c>
       <c r="J83" s="263">
-        <v>0.11768472667420256</v>
+        <v>0.11768472667345314</v>
       </c>
       <c r="K83" s="263">
-        <v>5.4015346300350107</v>
+        <v>5.4015346300328035</v>
       </c>
       <c r="L83" s="263">
-        <v>0.16505021300685302</v>
+        <v>0.1650502130038885</v>
       </c>
     </row>
     <row r="84" outlineLevel="2">
@@ -4956,10 +4956,10 @@
         <v>0</v>
       </c>
       <c r="K85" s="261">
-        <v>2.6057540405397264</v>
+        <v>2.6057540405419073</v>
       </c>
       <c r="L85" s="261">
-        <v>0.086764853170718484</v>
+        <v>0.086764853127098251</v>
       </c>
     </row>
     <row r="86" outlineLevel="2">
@@ -4994,10 +4994,10 @@
         <v>0</v>
       </c>
       <c r="K86" s="263">
-        <v>2.6057540405392303</v>
+        <v>2.605754040540591</v>
       </c>
       <c r="L86" s="263">
-        <v>0.0867648531642204</v>
+        <v>0.086764853137005785</v>
       </c>
     </row>
     <row r="87" outlineLevel="2">
@@ -5032,10 +5032,10 @@
         <v>0</v>
       </c>
       <c r="K87" s="261">
-        <v>1.4805648963558757</v>
+        <v>1.4805648963549496</v>
       </c>
       <c r="L87" s="261">
-        <v>0.036568996614469</v>
+        <v>0.036568996595943329</v>
       </c>
     </row>
     <row r="88" outlineLevel="2">
@@ -5043,25 +5043,25 @@
         <v>66</v>
       </c>
       <c r="B88" s="261">
-        <v>2427.7358038469861</v>
+        <v>2427.7358038468351</v>
       </c>
       <c r="C88" s="261">
-        <v>0.071825376010353478</v>
+        <v>0.071825376010264286</v>
       </c>
       <c r="D88" s="261">
-        <v>0.37958095788246771</v>
+        <v>0.3795809578824913</v>
       </c>
       <c r="E88" s="261">
-        <v>0.23810416584424224</v>
+        <v>0.23810416584416339</v>
       </c>
       <c r="F88" s="261">
-        <v>0.11432910627250587</v>
+        <v>0.11432910627063983</v>
       </c>
       <c r="G88" s="261">
-        <v>0.054166877277762211</v>
+        <v>0.054166877277765584</v>
       </c>
       <c r="H88" s="261">
-        <v>0.012235221595388904</v>
+        <v>0.012235221595389664</v>
       </c>
       <c r="I88" s="261">
         <v>0</v>
@@ -5070,10 +5070,10 @@
         <v>0</v>
       </c>
       <c r="K88" s="261">
-        <v>0.87024110846293323</v>
+        <v>0.870241108463081</v>
       </c>
       <c r="L88" s="261">
-        <v>0.013243077213703276</v>
+        <v>0.013243077215577234</v>
       </c>
     </row>
     <row r="89" outlineLevel="2">
@@ -5081,37 +5081,37 @@
         <v>67</v>
       </c>
       <c r="B89" s="261">
-        <v>56165.930306477785</v>
+        <v>56165.930306476956</v>
       </c>
       <c r="C89" s="261">
-        <v>0.056336863958924004</v>
+        <v>0.056336863958924836</v>
       </c>
       <c r="D89" s="261">
-        <v>0.45466784033139829</v>
+        <v>0.454667840331405</v>
       </c>
       <c r="E89" s="261">
-        <v>0.633572725361676</v>
+        <v>0.6335727253608433</v>
       </c>
       <c r="F89" s="261">
-        <v>0.592925756725303</v>
+        <v>0.59292575672537651</v>
       </c>
       <c r="G89" s="261">
-        <v>0.51627188687210224</v>
+        <v>0.51627188687295189</v>
       </c>
       <c r="H89" s="261">
-        <v>0.60122623016460464</v>
+        <v>0.601226230161051</v>
       </c>
       <c r="I89" s="261">
-        <v>0.095018602887518427</v>
+        <v>0.095018602888361878</v>
       </c>
       <c r="J89" s="261">
-        <v>0.0081647843354084454</v>
+        <v>0.0081647843354733379</v>
       </c>
       <c r="K89" s="261">
-        <v>2.9512028037428051</v>
+        <v>2.9512028037375373</v>
       </c>
       <c r="L89" s="261">
-        <v>0.042400442814817849</v>
+        <v>0.042400442848499913</v>
       </c>
     </row>
     <row r="90" outlineLevel="2">
@@ -5119,25 +5119,25 @@
         <v>68</v>
       </c>
       <c r="B90" s="261">
-        <v>669.0865817369903</v>
+        <v>669.086581736949</v>
       </c>
       <c r="C90" s="261">
-        <v>0.071825376011444189</v>
+        <v>0.07182537601144863</v>
       </c>
       <c r="D90" s="261">
-        <v>0.37958095788245355</v>
+        <v>0.37958095788171231</v>
       </c>
       <c r="E90" s="261">
-        <v>0.23810416584414273</v>
+        <v>0.23810416584483707</v>
       </c>
       <c r="F90" s="261">
-        <v>0.11432910627254922</v>
+        <v>0.11432910627187662</v>
       </c>
       <c r="G90" s="261">
-        <v>0.054166877277479882</v>
+        <v>0.05416687727833279</v>
       </c>
       <c r="H90" s="261">
-        <v>0.012235221596085765</v>
+        <v>0.012235221595321907</v>
       </c>
       <c r="I90" s="261">
         <v>0</v>
@@ -5146,10 +5146,10 @@
         <v>0</v>
       </c>
       <c r="K90" s="261">
-        <v>0.87024110846299019</v>
+        <v>0.87024110846151459</v>
       </c>
       <c r="L90" s="261">
-        <v>0.013243077221292681</v>
+        <v>0.013243077251877927</v>
       </c>
     </row>
     <row r="91" outlineLevel="2">
@@ -5157,37 +5157,37 @@
         <v>69</v>
       </c>
       <c r="B91" s="263">
-        <v>56835.016888214777</v>
+        <v>56835.016888213911</v>
       </c>
       <c r="C91" s="263">
-        <v>0.05651920147106</v>
+        <v>0.056519201471124873</v>
       </c>
       <c r="D91" s="263">
-        <v>0.45378388483598581</v>
+        <v>0.45378388483592874</v>
       </c>
       <c r="E91" s="263">
-        <v>0.628917097173984</v>
+        <v>0.62891709717316147</v>
       </c>
       <c r="F91" s="263">
-        <v>0.58729150843236</v>
+        <v>0.587291508432369</v>
       </c>
       <c r="G91" s="263">
-        <v>0.51083178536069462</v>
+        <v>0.51083178536159857</v>
       </c>
       <c r="H91" s="263">
-        <v>0.59429237138919189</v>
+        <v>0.59429237138568036</v>
       </c>
       <c r="I91" s="263">
-        <v>0.0939000024948683</v>
+        <v>0.093900002495701851</v>
       </c>
       <c r="J91" s="263">
-        <v>0.008068664936828113</v>
+        <v>0.0080686649368922458</v>
       </c>
       <c r="K91" s="263">
-        <v>2.9267048159942242</v>
+        <v>2.926704815988892</v>
       </c>
       <c r="L91" s="263">
-        <v>0.042057189603791872</v>
+        <v>0.042057189634517059</v>
       </c>
     </row>
     <row r="92" outlineLevel="2">
@@ -5195,37 +5195,37 @@
         <v>70</v>
       </c>
       <c r="B92" s="263">
-        <v>59262.75269206176</v>
+        <v>59262.752692060749</v>
       </c>
       <c r="C92" s="263">
-        <v>0.057146228503498805</v>
+        <v>0.057146228503499784</v>
       </c>
       <c r="D92" s="263">
-        <v>0.45074411543051063</v>
+        <v>0.45074411543045695</v>
       </c>
       <c r="E92" s="263">
-        <v>0.61290720052055847</v>
+        <v>0.61290720051977088</v>
       </c>
       <c r="F92" s="263">
-        <v>0.56791630722350261</v>
+        <v>0.56791630722351227</v>
       </c>
       <c r="G92" s="263">
-        <v>0.49212422121032329</v>
+        <v>0.49212422121119109</v>
       </c>
       <c r="H92" s="263">
-        <v>0.57044803547421186</v>
+        <v>0.57044803547078393</v>
       </c>
       <c r="I92" s="263">
-        <v>0.090053330045772817</v>
+        <v>0.090053330046633767</v>
       </c>
       <c r="J92" s="263">
-        <v>0.0077381270211405034</v>
+        <v>0.0077381270211406353</v>
       </c>
       <c r="K92" s="263">
-        <v>2.8424604914346117</v>
+        <v>2.8424604914295037</v>
       </c>
       <c r="L92" s="263">
-        <v>0.040876801432154275</v>
+        <v>0.040876801461620864</v>
       </c>
     </row>
     <row r="93" outlineLevel="2">
@@ -5347,37 +5347,37 @@
         <v>74</v>
       </c>
       <c r="B96" s="263">
-        <v>76608.564821065214</v>
+        <v>76608.56482106421</v>
       </c>
       <c r="C96" s="263">
-        <v>0.058175792876767</v>
+        <v>0.058175792876767767</v>
       </c>
       <c r="D96" s="263">
-        <v>0.46752736246032151</v>
+        <v>0.46752736246023269</v>
       </c>
       <c r="E96" s="263">
-        <v>0.73300061990132692</v>
+        <v>0.73300061990076659</v>
       </c>
       <c r="F96" s="263">
-        <v>0.43932794907971573</v>
+        <v>0.43932794907962647</v>
       </c>
       <c r="G96" s="263">
-        <v>0.38069680698872327</v>
+        <v>0.38069680698939307</v>
       </c>
       <c r="H96" s="263">
-        <v>0.441286440085938</v>
+        <v>0.44128644008328449</v>
       </c>
       <c r="I96" s="263">
-        <v>0.069663336469811737</v>
+        <v>0.069663336470477483</v>
       </c>
       <c r="J96" s="263">
-        <v>0.0059860501109906556</v>
+        <v>0.00598605011108571</v>
       </c>
       <c r="K96" s="263">
-        <v>2.5905456938575164</v>
+        <v>2.5905456938535614</v>
       </c>
       <c r="L96" s="263">
-        <v>0.042419599585764071</v>
+        <v>0.042419599604759779</v>
       </c>
     </row>
     <row r="97" outlineLevel="2">
@@ -5423,19 +5423,19 @@
         <v>76</v>
       </c>
       <c r="B98" s="261">
-        <v>6610.3496136915583</v>
+        <v>6610.3496136915483</v>
       </c>
       <c r="C98" s="261">
-        <v>0.013227212916810586</v>
+        <v>0.013227212916810605</v>
       </c>
       <c r="D98" s="261">
-        <v>0.1126797606153791</v>
+        <v>0.11267976061537928</v>
       </c>
       <c r="E98" s="261">
-        <v>1.7669056471360116</v>
+        <v>1.7669056471360143</v>
       </c>
       <c r="F98" s="261">
-        <v>1.5474387750464278</v>
+        <v>1.5474387750472556</v>
       </c>
       <c r="G98" s="261">
         <v>0</v>
@@ -5450,10 +5450,10 @@
         <v>0</v>
       </c>
       <c r="K98" s="261">
-        <v>3.4402600510579813</v>
+        <v>3.4402600510579862</v>
       </c>
       <c r="L98" s="261">
-        <v>0.14669469932051005</v>
+        <v>0.14669469935077931</v>
       </c>
     </row>
     <row r="99" outlineLevel="2">
@@ -5464,16 +5464,16 @@
         <v>4601.6209433511631</v>
       </c>
       <c r="C99" s="261">
-        <v>0.08575444758769879</v>
+        <v>0.085754447588884675</v>
       </c>
       <c r="D99" s="261">
         <v>0.51891043465996967</v>
       </c>
       <c r="E99" s="261">
-        <v>0.79943479044715238</v>
+        <v>0.79943479044814059</v>
       </c>
       <c r="F99" s="261">
-        <v>0.11484637124094174</v>
+        <v>0.1148463712420288</v>
       </c>
       <c r="G99" s="261">
         <v>0</v>
@@ -5508,7 +5508,7 @@
         <v>0.4959711024935704</v>
       </c>
       <c r="E100" s="261">
-        <v>0.901594484611559</v>
+        <v>0.90159448461284808</v>
       </c>
       <c r="F100" s="261">
         <v>0.146039024913881</v>
@@ -5540,16 +5540,16 @@
         <v>8305.66100023882</v>
       </c>
       <c r="C101" s="263">
-        <v>0.079952507098031131</v>
+        <v>0.079952507098688147</v>
       </c>
       <c r="D101" s="263">
         <v>0.50868027896006729</v>
       </c>
       <c r="E101" s="263">
-        <v>0.84499451162684147</v>
+        <v>0.844994511628046</v>
       </c>
       <c r="F101" s="263">
-        <v>0.1287572253777993</v>
+        <v>0.12875722537851106</v>
       </c>
       <c r="G101" s="263">
         <v>0</v>
@@ -5613,37 +5613,37 @@
         <v>81</v>
       </c>
       <c r="B103" s="263">
-        <v>94891.293904418271</v>
+        <v>94891.293904417267</v>
       </c>
       <c r="C103" s="263">
-        <v>0.056842254277644479</v>
+        <v>0.056842254277721757</v>
       </c>
       <c r="D103" s="263">
-        <v>0.44646346904496143</v>
+        <v>0.44646346904473611</v>
       </c>
       <c r="E103" s="263">
-        <v>0.8274234935984679</v>
+        <v>0.82742349359824663</v>
       </c>
       <c r="F103" s="263">
-        <v>0.49121426102339305</v>
+        <v>0.49121426102339827</v>
       </c>
       <c r="G103" s="263">
-        <v>0.30734785895903449</v>
+        <v>0.30734785895942113</v>
       </c>
       <c r="H103" s="263">
-        <v>0.35626367245063589</v>
+        <v>0.35626367244849272</v>
       </c>
       <c r="I103" s="263">
-        <v>0.056241284189621106</v>
+        <v>0.05624128419015844</v>
       </c>
       <c r="J103" s="263">
-        <v>0.0048327163544833905</v>
+        <v>0.0048327163545601182</v>
       </c>
       <c r="K103" s="263">
-        <v>2.5424974024836082</v>
+        <v>2.5424974024804148</v>
       </c>
       <c r="L103" s="263">
-        <v>0.050861219847516868</v>
+        <v>0.050861219862852761</v>
       </c>
     </row>
     <row r="104" outlineLevel="2">
@@ -5841,37 +5841,37 @@
         <v>49</v>
       </c>
       <c r="B109" s="263">
-        <v>112153.55805661147</v>
+        <v>112153.55805661112</v>
       </c>
       <c r="C109" s="263">
-        <v>0.050858588986229615</v>
+        <v>0.050858588986359525</v>
       </c>
       <c r="D109" s="263">
-        <v>0.38269886764937144</v>
+        <v>0.38269886764924288</v>
       </c>
       <c r="E109" s="263">
-        <v>0.77327348716380084</v>
+        <v>0.77327348716360855</v>
       </c>
       <c r="F109" s="263">
-        <v>0.4532275145766882</v>
+        <v>0.45322751457681937</v>
       </c>
       <c r="G109" s="263">
-        <v>0.28160964060253363</v>
+        <v>0.28160964060298865</v>
       </c>
       <c r="H109" s="263">
-        <v>0.43211715770912851</v>
+        <v>0.43211715770718362</v>
       </c>
       <c r="I109" s="263">
-        <v>0.069859296389232717</v>
+        <v>0.069859296389622183</v>
       </c>
       <c r="J109" s="263">
-        <v>0.010566490683961823</v>
+        <v>0.010566490684091604</v>
       </c>
       <c r="K109" s="263">
-        <v>2.450699984151254</v>
+        <v>2.450699984148407</v>
       </c>
       <c r="L109" s="263">
-        <v>0.052130450739404</v>
+        <v>0.052130450757569148</v>
       </c>
     </row>
     <row r="111">
@@ -5898,13 +5898,13 @@
         <v>40682.7667188486</v>
       </c>
       <c r="C112" s="261">
-        <v>-0.0014906508760909715</v>
+        <v>-0.0014906508760015483</v>
       </c>
       <c r="D112" s="261">
-        <v>0.4645873878102017</v>
+        <v>0.46458738781011227</v>
       </c>
       <c r="E112" s="261">
-        <v>0.31262325143573266</v>
+        <v>0.31262325143698455</v>
       </c>
       <c r="F112" s="261">
         <v>0.13582722668397754</v>
@@ -5913,19 +5913,19 @@
         <v>0.023362355187613714</v>
       </c>
       <c r="H112" s="261">
-        <v>0.032828400095755807</v>
+        <v>0.032828400094593306</v>
       </c>
       <c r="I112" s="261">
-        <v>0.0079958427839299743</v>
+        <v>0.0079958427850924749</v>
       </c>
       <c r="J112" s="261">
-        <v>0.00063641172751272067</v>
+        <v>0.00063641172635022045</v>
       </c>
       <c r="K112" s="261">
-        <v>0.97612276173563028</v>
+        <v>0.97612276173688217</v>
       </c>
       <c r="L112" s="261">
-        <v>0.04976320005410062</v>
+        <v>0.049763200079139085</v>
       </c>
     </row>
     <row r="113" outlineLevel="2">
@@ -5933,37 +5933,37 @@
         <v>89</v>
       </c>
       <c r="B113" s="261">
-        <v>1603.51384266222</v>
+        <v>1603.5138426624299</v>
       </c>
       <c r="C113" s="261">
-        <v>0.059775246723707362</v>
+        <v>0.059775246726819074</v>
       </c>
       <c r="D113" s="261">
-        <v>0.098052255538327041</v>
+        <v>0.0980522555383851</v>
       </c>
       <c r="E113" s="261">
-        <v>0.23234510189607446</v>
+        <v>0.23234510189604404</v>
       </c>
       <c r="F113" s="261">
-        <v>0.30042123951685873</v>
+        <v>0.30042123951993893</v>
       </c>
       <c r="G113" s="261">
-        <v>0.39848825124529691</v>
+        <v>0.39848825124205428</v>
       </c>
       <c r="H113" s="261">
-        <v>0.85922530062323021</v>
+        <v>0.85922530062311775</v>
       </c>
       <c r="I113" s="261">
-        <v>0.7594410897901871</v>
+        <v>0.75944108979001679</v>
       </c>
       <c r="J113" s="261">
-        <v>0.44301366157258942</v>
+        <v>0.443013661569341</v>
       </c>
       <c r="K113" s="261">
-        <v>3.150830558613646</v>
+        <v>3.1508305586163532</v>
       </c>
       <c r="L113" s="261">
-        <v>0.42210980247959706</v>
+        <v>0.422109802419987</v>
       </c>
     </row>
     <row r="114" outlineLevel="2">
@@ -5971,37 +5971,37 @@
         <v>90</v>
       </c>
       <c r="B114" s="261">
-        <v>24018.829166609</v>
+        <v>24018.829166610798</v>
       </c>
       <c r="C114" s="261">
-        <v>0.0715460198488943</v>
+        <v>0.071546019848888948</v>
       </c>
       <c r="D114" s="261">
-        <v>0.12790840595883488</v>
+        <v>0.12790840595890105</v>
       </c>
       <c r="E114" s="261">
-        <v>0.2562094855712761</v>
+        <v>0.25620948557322593</v>
       </c>
       <c r="F114" s="261">
-        <v>0.26441780129861137</v>
+        <v>0.26441780130056064</v>
       </c>
       <c r="G114" s="261">
-        <v>0.26866880363889373</v>
+        <v>0.2686688036389494</v>
       </c>
       <c r="H114" s="261">
-        <v>0.35147053861754685</v>
+        <v>0.35147053861744482</v>
       </c>
       <c r="I114" s="261">
-        <v>0.15008980731503846</v>
+        <v>0.15008980731502725</v>
       </c>
       <c r="J114" s="261">
-        <v>0.020218653795779196</v>
+        <v>0.020218653795777683</v>
       </c>
       <c r="K114" s="261">
-        <v>1.5105501255838925</v>
+        <v>1.5105501255859</v>
       </c>
       <c r="L114" s="261">
-        <v>0.11022714261544346</v>
+        <v>0.11022714257605466</v>
       </c>
     </row>
     <row r="115" outlineLevel="2">
@@ -6009,37 +6009,37 @@
         <v>91</v>
       </c>
       <c r="B115" s="261">
-        <v>8628.819204122281</v>
+        <v>8628.8192041225811</v>
       </c>
       <c r="C115" s="261">
-        <v>0.081428086524852089</v>
+        <v>0.081428086525376267</v>
       </c>
       <c r="D115" s="261">
-        <v>0.11337497771411011</v>
+        <v>0.11337497771389536</v>
       </c>
       <c r="E115" s="261">
-        <v>0.18466358412161552</v>
+        <v>0.1846635841221361</v>
       </c>
       <c r="F115" s="261">
-        <v>0.14824225484446782</v>
+        <v>0.14824225484456804</v>
       </c>
       <c r="G115" s="261">
-        <v>0.11205271220351401</v>
+        <v>0.11205271220351011</v>
       </c>
       <c r="H115" s="261">
-        <v>0.08987626235980245</v>
+        <v>0.089876262359272319</v>
       </c>
       <c r="I115" s="261">
-        <v>0.019104203557341035</v>
+        <v>0.019104203557340368</v>
       </c>
       <c r="J115" s="261">
-        <v>0.00065100610774589183</v>
+        <v>0.00065100610785127119</v>
       </c>
       <c r="K115" s="261">
-        <v>0.74940144215905657</v>
+        <v>0.749401442159663</v>
       </c>
       <c r="L115" s="261">
-        <v>0.030257953816443143</v>
+        <v>0.030257953803793852</v>
       </c>
     </row>
     <row r="116" outlineLevel="2">
@@ -6047,37 +6047,37 @@
         <v>92</v>
       </c>
       <c r="B116" s="261">
-        <v>14945.5606565359</v>
+        <v>14945.5606565376</v>
       </c>
       <c r="C116" s="261">
-        <v>0.091363209930996947</v>
+        <v>0.091363209930925685</v>
       </c>
       <c r="D116" s="261">
-        <v>0.45811736059941427</v>
+        <v>0.45811736059936214</v>
       </c>
       <c r="E116" s="261">
-        <v>0.62944685181389681</v>
+        <v>0.62944685181717219</v>
       </c>
       <c r="F116" s="261">
-        <v>0.37330545504557167</v>
+        <v>0.37330545504218227</v>
       </c>
       <c r="G116" s="261">
-        <v>0.20162909567608262</v>
+        <v>0.20162909567612053</v>
       </c>
       <c r="H116" s="261">
-        <v>0.098613007659610633</v>
+        <v>0.09861300765966026</v>
       </c>
       <c r="I116" s="261">
-        <v>0.010647568251643442</v>
+        <v>0.010647568251703085</v>
       </c>
       <c r="J116" s="261">
-        <v>7.7879560728933138E-05</v>
+        <v>7.7879557442817117E-05</v>
       </c>
       <c r="K116" s="261">
-        <v>1.8632043291745903</v>
+        <v>1.8632043291745</v>
       </c>
       <c r="L116" s="261">
-        <v>0.07702694361761056</v>
+        <v>0.07702694361516764</v>
       </c>
     </row>
     <row r="117" outlineLevel="1">
@@ -6085,37 +6085,37 @@
         <v>93</v>
       </c>
       <c r="B117" s="263">
-        <v>89879.489588777986</v>
+        <v>89879.489588782017</v>
       </c>
       <c r="C117" s="263">
-        <v>0.042520945680385114</v>
+        <v>0.042520945680464155</v>
       </c>
       <c r="D117" s="263">
-        <v>0.33328239559684819</v>
+        <v>0.33328239559699518</v>
       </c>
       <c r="E117" s="263">
-        <v>0.33651352699272774</v>
+        <v>0.33651352699465553</v>
       </c>
       <c r="F117" s="263">
-        <v>0.213808267232375</v>
+        <v>0.21380826723244636</v>
       </c>
       <c r="G117" s="263">
-        <v>0.13376666133302134</v>
+        <v>0.13376666133277249</v>
       </c>
       <c r="H117" s="263">
-        <v>0.14913962460164551</v>
+        <v>0.1491396246011531</v>
       </c>
       <c r="I117" s="263">
-        <v>0.06088184711700808</v>
+        <v>0.060881847117491061</v>
       </c>
       <c r="J117" s="263">
-        <v>0.01367029667719097</v>
+        <v>0.013670296676137976</v>
       </c>
       <c r="K117" s="263">
-        <v>1.2834797330955499</v>
+        <v>1.2834797330967065</v>
       </c>
       <c r="L117" s="263">
-        <v>0.075225079499422587</v>
+        <v>0.075225079494562072</v>
       </c>
     </row>
     <row r="118" outlineLevel="2">
@@ -6199,37 +6199,37 @@
         <v>87</v>
       </c>
       <c r="B120" s="263">
-        <v>90250.489588777986</v>
+        <v>90250.489588782017</v>
       </c>
       <c r="C120" s="263">
-        <v>0.04234615138376354</v>
+        <v>0.042346151383842269</v>
       </c>
       <c r="D120" s="263">
-        <v>0.33191234464942593</v>
+        <v>0.33191234464957237</v>
       </c>
       <c r="E120" s="263">
-        <v>0.3351301935716775</v>
+        <v>0.33513019357359741</v>
       </c>
       <c r="F120" s="263">
-        <v>0.21292934826468141</v>
+        <v>0.21292934826475252</v>
       </c>
       <c r="G120" s="263">
-        <v>0.13321677587998199</v>
+        <v>0.13321677587973416</v>
       </c>
       <c r="H120" s="263">
-        <v>0.14852654426292022</v>
+        <v>0.14852654426242987</v>
       </c>
       <c r="I120" s="263">
-        <v>0.060631575175178982</v>
+        <v>0.060631575175659994</v>
       </c>
       <c r="J120" s="263">
-        <v>0.013614101081019174</v>
+        <v>0.013614101079970511</v>
       </c>
       <c r="K120" s="263">
-        <v>1.2782036289641694</v>
+        <v>1.2782036289653216</v>
       </c>
       <c r="L120" s="263">
-        <v>0.07491584567009435</v>
+        <v>0.074915845665253819</v>
       </c>
     </row>
     <row r="122">
@@ -6253,37 +6253,37 @@
         <v>95</v>
       </c>
       <c r="B123" s="263">
-        <v>21903.068467833476</v>
+        <v>21903.068467829104</v>
       </c>
       <c r="C123" s="263">
-        <v>0.085933659054201708</v>
+        <v>0.085933659054883232</v>
       </c>
       <c r="D123" s="263">
-        <v>0.59196217575546872</v>
+        <v>0.59196217575459031</v>
       </c>
       <c r="E123" s="263">
-        <v>2.5786208436221241</v>
+        <v>2.578620843613753</v>
       </c>
       <c r="F123" s="263">
-        <v>1.4433639965398435</v>
+        <v>1.4433639965405469</v>
       </c>
       <c r="G123" s="263">
-        <v>0.89305495989025341</v>
+        <v>0.89305495989350447</v>
       </c>
       <c r="H123" s="263">
-        <v>1.6006379859160564</v>
+        <v>1.6006379859085695</v>
       </c>
       <c r="I123" s="263">
-        <v>0.1078816565247612</v>
+        <v>0.1078816565243675</v>
       </c>
       <c r="J123" s="263">
-        <v>-0.0019910343409254459</v>
+        <v>-0.0019910343361921505</v>
       </c>
       <c r="K123" s="263">
-        <v>7.2819121155517195</v>
+        <v>7.2819121155334079</v>
       </c>
       <c r="L123" s="263">
-        <v>-0.04175562056555733</v>
+        <v>-0.041755620455943311</v>
       </c>
     </row>
   </sheetData>

</xml_diff>